<commit_message>
1.3.0 Started tests. Fixed a few issues with address. Added security tags to resources.
</commit_message>
<xml_diff>
--- a/samples/Congenital_Hyperthyrodism/Congenital_Hyperthyrodism_Fhir_Cohort_Import_Template.xlsx
+++ b/samples/Congenital_Hyperthyrodism/Congenital_Hyperthyrodism_Fhir_Cohort_Import_Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mriley7/workspace/FHIRSheets/samples/Congenital_Hypersyphilis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mriley7/workspace/FHIRSheets/samples/Congenital_Hyperthyrodism/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DDCAFB3A-0ABE-5847-8FDA-73336D3A7C34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F64A4E3-A938-CB4A-8DED-12671A1AA45B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17820" activeTab="4" xr2:uid="{B7CAF98F-F4CF-4673-A736-BDE9BA8D985C}"/>
+    <workbookView xWindow="-36880" yWindow="-1460" windowWidth="38400" windowHeight="19880" activeTab="1" xr2:uid="{B7CAF98F-F4CF-4673-A736-BDE9BA8D985C}"/>
   </bookViews>
   <sheets>
     <sheet name="How To Use This Workbook" sheetId="6" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1001" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="971" uniqueCount="421">
   <si>
     <t>How To Use This Workbook</t>
   </si>
@@ -705,9 +705,6 @@
     <t>http://terminology.hl7.org/CodeSystem/v3-ActCode^IMP^inpatient encounter</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/sid/icd-10^O80^full-term uncomplicated delivery</t>
-  </si>
-  <si>
     <t>http://terminology.hl7.org/CodeSystem/discharge-disposition^home^Home</t>
   </si>
   <si>
@@ -726,15 +723,6 @@
     <t>completed</t>
   </si>
   <si>
-    <t>http://www.ama-assn.org/go/cpt^92558^Audiologic Function Tests</t>
-  </si>
-  <si>
-    <t>http://www.ama-assn.org/go/cpt^87496^Infectious agent detection by nucleic acid (DNA or RNA)</t>
-  </si>
-  <si>
-    <t>http://www.ama-assn.org/go/cpt^70551^Magnetic resonance (eg, proton) imaging, brain (including brain stem)</t>
-  </si>
-  <si>
     <t>http://terminology.hl7.org/CodeSystem/condition-clinical^active^Active</t>
   </si>
   <si>
@@ -744,9 +732,6 @@
     <t>http://hl7.org/fhir/us/core/CodeSystem/condition-category^health-concern^Health Concern</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/sid/icd-10^E03.1^congenital hypothyroidism without goiter.</t>
-  </si>
-  <si>
     <t>active</t>
   </si>
   <si>
@@ -1308,7 +1293,19 @@
     <t>final</t>
   </si>
   <si>
-    <t>FollowupDiagnosis</t>
+    <t>http://hl7.org/fhir/sid/icd-10^E03.1^congenital hypothyroidism without goitre</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/sid/icd-10^O80^Single spontaneous delivery</t>
+  </si>
+  <si>
+    <t>http://www.ama-assn.org/go/cpt^92558^Automated evoked otoacoustic emissions screening</t>
+  </si>
+  <si>
+    <t>http://www.ama-assn.org/go/cpt^87496^Cytomegalovirus detection by amplified nucleic acid probe technique</t>
+  </si>
+  <si>
+    <t>http://www.ama-assn.org/go/cpt^70551^MRI scan of brain without contrast</t>
   </si>
 </sst>
 </file>
@@ -2156,23 +2153,23 @@
     <xf numFmtId="0" fontId="6" fillId="21" borderId="0" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="21" borderId="0" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -2537,36 +2534,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A1" s="112" t="s">
+      <c r="A1" s="114" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="112"/>
+      <c r="B1" s="114"/>
     </row>
     <row r="2" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="110" t="s">
+      <c r="A2" s="111" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="110"/>
-      <c r="C2" s="110"/>
+      <c r="B2" s="111"/>
+      <c r="C2" s="111"/>
     </row>
     <row r="3" spans="1:3" ht="103.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="111" t="s">
+      <c r="A3" s="113" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="111"/>
+      <c r="B3" s="113"/>
     </row>
     <row r="4" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="109" t="s">
+      <c r="A4" s="112" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="109"/>
-      <c r="C4" s="109"/>
+      <c r="B4" s="112"/>
+      <c r="C4" s="112"/>
     </row>
     <row r="5" spans="1:3" ht="41" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="114" t="s">
+      <c r="A5" s="110" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="114"/>
+      <c r="B5" s="110"/>
     </row>
     <row r="6" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="97" t="s">
@@ -2601,35 +2598,35 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="110" t="s">
+      <c r="A10" s="111" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="110"/>
-      <c r="C10" s="110"/>
+      <c r="B10" s="111"/>
+      <c r="C10" s="111"/>
     </row>
     <row r="11" spans="1:3" ht="37.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="111" t="s">
+      <c r="A11" s="113" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="111"/>
+      <c r="B11" s="113"/>
     </row>
     <row r="12" spans="1:3" ht="37.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="113" t="s">
+      <c r="A12" s="109" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="113"/>
+      <c r="B12" s="109"/>
     </row>
     <row r="13" spans="1:3" ht="37.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="113" t="s">
+      <c r="A13" s="109" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="113"/>
+      <c r="B13" s="109"/>
     </row>
     <row r="14" spans="1:3" ht="37.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="113" t="s">
+      <c r="A14" s="109" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="113"/>
+      <c r="B14" s="109"/>
     </row>
     <row r="15" spans="1:3" ht="36" x14ac:dyDescent="0.2">
       <c r="A15" s="108" t="s">
@@ -2686,16 +2683,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A11:B11"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A6" location="ResourceDefinitions!A1" display="ResourceDefinitions" xr:uid="{21E4973D-DCF1-4F08-A5DE-B12BC88A3D35}"/>
@@ -2710,10 +2707,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E456F74-46A1-4B4C-AEC2-C20EF6B49B86}">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2837,15 +2834,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>421</v>
-      </c>
-      <c r="B11" t="s">
-        <v>51</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>52</v>
-      </c>
+      <c r="C11" s="7"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C12" s="7"/>
@@ -2894,18 +2883,14 @@
     </row>
     <row r="27" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C27" s="7"/>
-    </row>
-    <row r="28" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C28" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C9" r:id="rId1" xr:uid="{F970F9D3-065F-4CA4-BBB5-A7ABA7E8E290}"/>
     <hyperlink ref="C10" r:id="rId2" xr:uid="{CBBC0D42-CF64-457D-BE5D-13EF48C83D96}"/>
-    <hyperlink ref="C11" r:id="rId3" xr:uid="{025056E8-2A78-1B47-AC56-29498E509A8E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId4"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -2914,7 +2899,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:C12"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3061,11 +3046,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFB4DC11-02AF-44A1-9E33-056BEEEC10B1}">
-  <dimension ref="A1:BR16"/>
+  <dimension ref="A1:BM16"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="BD1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BG7" sqref="BG7"/>
+      <pane xSplit="1" topLeftCell="AY1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AY8" sqref="AY8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="30" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3077,7 +3062,7 @@
     <col min="49" max="53" width="29.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:70" ht="52.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:65" ht="52.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
         <v>64</v>
       </c>
@@ -3252,30 +3237,15 @@
       <c r="BF1" s="82" t="s">
         <v>53</v>
       </c>
-      <c r="BG1" s="81" t="s">
-        <v>421</v>
-      </c>
-      <c r="BH1" s="81" t="s">
-        <v>421</v>
-      </c>
-      <c r="BI1" s="81" t="s">
-        <v>421</v>
-      </c>
-      <c r="BJ1" s="81" t="s">
-        <v>421</v>
-      </c>
-      <c r="BK1" s="81" t="s">
-        <v>421</v>
-      </c>
-      <c r="BL1" s="12"/>
+      <c r="BG1" s="12"/>
+      <c r="BH1" s="11"/>
+      <c r="BI1" s="11"/>
+      <c r="BJ1" s="11"/>
+      <c r="BK1" s="11"/>
+      <c r="BL1" s="11"/>
       <c r="BM1" s="11"/>
-      <c r="BN1" s="11"/>
-      <c r="BO1" s="11"/>
-      <c r="BP1" s="11"/>
-      <c r="BQ1" s="11"/>
-      <c r="BR1" s="11"/>
-    </row>
-    <row r="2" spans="1:70" s="2" customFormat="1" ht="52.25" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:65" s="2" customFormat="1" ht="52.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="28" t="s">
         <v>66</v>
       </c>
@@ -3450,30 +3420,15 @@
       <c r="BF2" s="63" t="s">
         <v>117</v>
       </c>
-      <c r="BG2" s="61" t="s">
-        <v>108</v>
-      </c>
-      <c r="BH2" s="61" t="s">
-        <v>109</v>
-      </c>
-      <c r="BI2" s="61" t="s">
-        <v>286</v>
-      </c>
-      <c r="BJ2" s="61" t="s">
-        <v>111</v>
-      </c>
-      <c r="BK2" s="61" t="s">
-        <v>112</v>
-      </c>
+      <c r="BG2" s="12"/>
+      <c r="BH2" s="12"/>
+      <c r="BI2" s="12"/>
+      <c r="BJ2" s="12"/>
+      <c r="BK2" s="12"/>
       <c r="BL2" s="12"/>
       <c r="BM2" s="12"/>
-      <c r="BN2" s="12"/>
-      <c r="BO2" s="12"/>
-      <c r="BP2" s="12"/>
-      <c r="BQ2" s="12"/>
-      <c r="BR2" s="12"/>
-    </row>
-    <row r="3" spans="1:70" ht="52.25" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:65" ht="52.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="30" t="s">
         <v>118</v>
       </c>
@@ -3646,30 +3601,15 @@
       <c r="BF3" s="63" t="s">
         <v>121</v>
       </c>
-      <c r="BG3" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="BH3" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="BI3" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="BJ3" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="BK3" s="61" t="s">
-        <v>125</v>
-      </c>
+      <c r="BG3" s="12"/>
+      <c r="BH3" s="12"/>
+      <c r="BI3" s="12"/>
+      <c r="BJ3" s="12"/>
+      <c r="BK3" s="12"/>
       <c r="BL3" s="12"/>
       <c r="BM3" s="12"/>
-      <c r="BN3" s="12"/>
-      <c r="BO3" s="12"/>
-      <c r="BP3" s="12"/>
-      <c r="BQ3" s="12"/>
-      <c r="BR3" s="12"/>
-    </row>
-    <row r="4" spans="1:70" ht="52.25" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:65" ht="52.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="31" t="s">
         <v>126</v>
       </c>
@@ -3784,26 +3724,15 @@
       </c>
       <c r="BE4" s="63"/>
       <c r="BF4" s="63"/>
-      <c r="BG4" s="62" t="s">
-        <v>141</v>
-      </c>
-      <c r="BH4" s="62" t="s">
-        <v>142</v>
-      </c>
-      <c r="BI4" s="62" t="s">
-        <v>143</v>
-      </c>
-      <c r="BJ4" s="62"/>
-      <c r="BK4" s="62"/>
+      <c r="BG4" s="1"/>
+      <c r="BH4" s="1"/>
+      <c r="BI4" s="1"/>
+      <c r="BJ4" s="1"/>
+      <c r="BK4" s="1"/>
       <c r="BL4" s="1"/>
       <c r="BM4" s="1"/>
-      <c r="BN4" s="1"/>
-      <c r="BO4" s="1"/>
-      <c r="BP4" s="1"/>
-      <c r="BQ4" s="1"/>
-      <c r="BR4" s="1"/>
-    </row>
-    <row r="5" spans="1:70" ht="65.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:65" ht="65.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="26" t="s">
         <v>147</v>
       </c>
@@ -3948,28 +3877,15 @@
       <c r="BF5" s="63" t="s">
         <v>55</v>
       </c>
-      <c r="BG5" s="61" t="s">
-        <v>348</v>
-      </c>
-      <c r="BH5" s="61" t="s">
-        <v>348</v>
-      </c>
-      <c r="BI5" s="61" t="s">
-        <v>348</v>
-      </c>
-      <c r="BJ5" s="61" t="s">
-        <v>348</v>
-      </c>
-      <c r="BK5" s="61"/>
+      <c r="BG5" s="12"/>
+      <c r="BH5" s="12"/>
+      <c r="BI5" s="12"/>
+      <c r="BJ5" s="12"/>
+      <c r="BK5" s="12"/>
       <c r="BL5" s="12"/>
       <c r="BM5" s="12"/>
-      <c r="BN5" s="12"/>
-      <c r="BO5" s="12"/>
-      <c r="BP5" s="12"/>
-      <c r="BQ5" s="12"/>
-      <c r="BR5" s="12"/>
-    </row>
-    <row r="6" spans="1:70" s="2" customFormat="1" ht="52.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:65" s="2" customFormat="1" ht="52.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="33" t="s">
         <v>149</v>
       </c>
@@ -4144,30 +4060,15 @@
       <c r="BF6" s="88" t="s">
         <v>200</v>
       </c>
-      <c r="BG6" s="88" t="s">
-        <v>191</v>
-      </c>
-      <c r="BH6" s="88" t="s">
-        <v>192</v>
-      </c>
-      <c r="BI6" s="88" t="s">
-        <v>193</v>
-      </c>
-      <c r="BJ6" s="88" t="s">
-        <v>194</v>
-      </c>
-      <c r="BK6" s="88" t="s">
-        <v>195</v>
-      </c>
-      <c r="BL6" s="13"/>
-      <c r="BM6" s="13"/>
-      <c r="BN6" s="13"/>
-      <c r="BO6" s="13"/>
-      <c r="BP6" s="13"/>
-      <c r="BQ6" s="14"/>
-      <c r="BR6" s="14"/>
-    </row>
-    <row r="7" spans="1:70" s="2" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="BG6" s="13"/>
+      <c r="BH6" s="13"/>
+      <c r="BI6" s="13"/>
+      <c r="BJ6" s="13"/>
+      <c r="BK6" s="13"/>
+      <c r="BL6" s="14"/>
+      <c r="BM6" s="14"/>
+    </row>
+    <row r="7" spans="1:65" s="2" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A7" s="115"/>
       <c r="B7" s="103"/>
       <c r="C7" s="99" t="s">
@@ -4240,7 +4141,7 @@
         <v>219</v>
       </c>
       <c r="Z7" s="100" t="s">
-        <v>220</v>
+        <v>417</v>
       </c>
       <c r="AA7" s="102">
         <v>43591.459293981483</v>
@@ -4249,7 +4150,7 @@
         <v>43591.671261574076</v>
       </c>
       <c r="AC7" s="100" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AD7" s="99" t="s">
         <v>217</v>
@@ -4258,10 +4159,10 @@
         <v>4567</v>
       </c>
       <c r="AF7" s="100" t="s">
+        <v>221</v>
+      </c>
+      <c r="AG7" s="99" t="s">
         <v>222</v>
-      </c>
-      <c r="AG7" s="99" t="s">
-        <v>223</v>
       </c>
       <c r="AH7" s="99" t="s">
         <v>209</v>
@@ -4273,78 +4174,73 @@
         <v>211</v>
       </c>
       <c r="AK7" s="99" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="AL7" s="99" t="s">
         <v>213</v>
       </c>
       <c r="AM7" s="99" t="s">
+        <v>224</v>
+      </c>
+      <c r="AN7" s="99" t="s">
         <v>225</v>
       </c>
-      <c r="AN7" s="99" t="s">
-        <v>226</v>
-      </c>
       <c r="AO7" s="100" t="s">
-        <v>227</v>
+        <v>418</v>
       </c>
       <c r="AP7" s="101">
         <v>43592</v>
       </c>
       <c r="AQ7" s="99" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AR7" s="100" t="s">
-        <v>228</v>
+        <v>419</v>
       </c>
       <c r="AS7" s="101">
         <v>43593</v>
       </c>
       <c r="AT7" s="99" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AU7" s="100" t="s">
-        <v>229</v>
+        <v>420</v>
       </c>
       <c r="AV7" s="101">
         <v>43205</v>
       </c>
       <c r="AW7" s="100" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="AX7" s="100" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="AY7" s="100" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="AZ7" s="100" t="s">
-        <v>233</v>
+        <v>416</v>
       </c>
       <c r="BA7" s="101">
         <v>43591</v>
       </c>
       <c r="BB7" s="99" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="BC7" s="99" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="BD7" s="100" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="BE7" s="102">
         <v>43591</v>
       </c>
       <c r="BF7" s="99" t="s">
-        <v>237</v>
-      </c>
-      <c r="BG7" s="16"/>
-      <c r="BH7" s="16"/>
-      <c r="BI7" s="16"/>
-      <c r="BJ7" s="16"/>
-      <c r="BK7" s="16"/>
-    </row>
-    <row r="8" spans="1:70" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="8" spans="1:65" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="115"/>
       <c r="B8" s="103"/>
       <c r="C8" s="104"/>
@@ -4353,13 +4249,8 @@
       <c r="AY8" s="92"/>
       <c r="AZ8" s="92"/>
       <c r="BA8" s="92"/>
-      <c r="BG8" s="92"/>
-      <c r="BH8" s="92"/>
-      <c r="BI8" s="92"/>
-      <c r="BJ8" s="92"/>
-      <c r="BK8" s="92"/>
-    </row>
-    <row r="9" spans="1:70" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:65" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="115"/>
       <c r="B9" s="103"/>
       <c r="C9" s="104"/>
@@ -4368,13 +4259,8 @@
       <c r="AY9" s="92"/>
       <c r="AZ9" s="92"/>
       <c r="BA9" s="92"/>
-      <c r="BG9" s="92"/>
-      <c r="BH9" s="92"/>
-      <c r="BI9" s="92"/>
-      <c r="BJ9" s="92"/>
-      <c r="BK9" s="92"/>
-    </row>
-    <row r="10" spans="1:70" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:65" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="115"/>
       <c r="B10" s="103"/>
       <c r="C10" s="104"/>
@@ -4383,13 +4269,8 @@
       <c r="AY10" s="92"/>
       <c r="AZ10" s="92"/>
       <c r="BA10" s="92"/>
-      <c r="BG10" s="92"/>
-      <c r="BH10" s="92"/>
-      <c r="BI10" s="92"/>
-      <c r="BJ10" s="92"/>
-      <c r="BK10" s="92"/>
-    </row>
-    <row r="11" spans="1:70" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:65" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="115"/>
       <c r="B11" s="103"/>
       <c r="C11" s="104"/>
@@ -4398,13 +4279,8 @@
       <c r="AY11" s="92"/>
       <c r="AZ11" s="92"/>
       <c r="BA11" s="92"/>
-      <c r="BG11" s="92"/>
-      <c r="BH11" s="92"/>
-      <c r="BI11" s="92"/>
-      <c r="BJ11" s="92"/>
-      <c r="BK11" s="92"/>
-    </row>
-    <row r="12" spans="1:70" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:65" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="115"/>
       <c r="B12" s="103"/>
       <c r="C12" s="104"/>
@@ -4413,13 +4289,8 @@
       <c r="AY12" s="92"/>
       <c r="AZ12" s="92"/>
       <c r="BA12" s="92"/>
-      <c r="BG12" s="92"/>
-      <c r="BH12" s="92"/>
-      <c r="BI12" s="92"/>
-      <c r="BJ12" s="92"/>
-      <c r="BK12" s="92"/>
-    </row>
-    <row r="13" spans="1:70" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:65" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="115"/>
       <c r="B13" s="103"/>
       <c r="C13" s="104"/>
@@ -4428,13 +4299,8 @@
       <c r="AY13" s="92"/>
       <c r="AZ13" s="92"/>
       <c r="BA13" s="92"/>
-      <c r="BG13" s="92"/>
-      <c r="BH13" s="92"/>
-      <c r="BI13" s="92"/>
-      <c r="BJ13" s="92"/>
-      <c r="BK13" s="92"/>
-    </row>
-    <row r="14" spans="1:70" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:65" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="115"/>
       <c r="B14" s="103"/>
       <c r="C14" s="104"/>
@@ -4443,13 +4309,8 @@
       <c r="AY14" s="92"/>
       <c r="AZ14" s="92"/>
       <c r="BA14" s="92"/>
-      <c r="BG14" s="92"/>
-      <c r="BH14" s="92"/>
-      <c r="BI14" s="92"/>
-      <c r="BJ14" s="92"/>
-      <c r="BK14" s="92"/>
-    </row>
-    <row r="15" spans="1:70" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:65" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="115"/>
       <c r="B15" s="103"/>
       <c r="C15" s="104"/>
@@ -4458,13 +4319,8 @@
       <c r="AY15" s="92"/>
       <c r="AZ15" s="92"/>
       <c r="BA15" s="92"/>
-      <c r="BG15" s="92"/>
-      <c r="BH15" s="92"/>
-      <c r="BI15" s="92"/>
-      <c r="BJ15" s="92"/>
-      <c r="BK15" s="92"/>
-    </row>
-    <row r="16" spans="1:70" s="2" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:65" s="2" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="116"/>
       <c r="B16" s="105"/>
       <c r="C16" s="106"/>
@@ -4518,11 +4374,6 @@
       <c r="AY16" s="21"/>
       <c r="AZ16" s="21"/>
       <c r="BA16" s="21"/>
-      <c r="BG16" s="21"/>
-      <c r="BH16" s="21"/>
-      <c r="BI16" s="21"/>
-      <c r="BJ16" s="21"/>
-      <c r="BK16" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4570,9 +4421,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D010D53-A2B8-4D7D-8239-2883E618B035}">
   <dimension ref="A1:DQ16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="DI1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DQ5" sqref="DQ5"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="DB1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="X1" sqref="X1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="30" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4593,7 +4444,7 @@
         <v>64</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C1" s="69"/>
       <c r="D1" s="70"/>
@@ -4783,67 +4634,67 @@
         <v>85</v>
       </c>
       <c r="W2" s="35" t="s">
+        <v>234</v>
+      </c>
+      <c r="X2" s="37" t="s">
+        <v>235</v>
+      </c>
+      <c r="Y2" s="37" t="s">
+        <v>236</v>
+      </c>
+      <c r="Z2" s="37" t="s">
+        <v>237</v>
+      </c>
+      <c r="AA2" s="37" t="s">
+        <v>238</v>
+      </c>
+      <c r="AB2" s="39" t="s">
         <v>239</v>
       </c>
-      <c r="X2" s="37" t="s">
+      <c r="AC2" s="39" t="s">
         <v>240</v>
       </c>
-      <c r="Y2" s="37" t="s">
+      <c r="AD2" s="39" t="s">
         <v>241</v>
       </c>
-      <c r="Z2" s="37" t="s">
+      <c r="AE2" s="41" t="s">
         <v>242</v>
       </c>
-      <c r="AA2" s="37" t="s">
+      <c r="AF2" s="41" t="s">
         <v>243</v>
       </c>
-      <c r="AB2" s="39" t="s">
+      <c r="AG2" s="41" t="s">
         <v>244</v>
       </c>
-      <c r="AC2" s="39" t="s">
+      <c r="AH2" s="41" t="s">
         <v>245</v>
       </c>
-      <c r="AD2" s="39" t="s">
+      <c r="AI2" s="41" t="s">
         <v>246</v>
       </c>
-      <c r="AE2" s="41" t="s">
+      <c r="AJ2" s="43" t="s">
         <v>247</v>
       </c>
-      <c r="AF2" s="41" t="s">
+      <c r="AK2" s="43" t="s">
         <v>248</v>
       </c>
-      <c r="AG2" s="41" t="s">
+      <c r="AL2" s="43" t="s">
         <v>249</v>
       </c>
-      <c r="AH2" s="41" t="s">
+      <c r="AM2" s="43" t="s">
         <v>250</v>
       </c>
-      <c r="AI2" s="41" t="s">
+      <c r="AN2" s="43" t="s">
         <v>251</v>
       </c>
-      <c r="AJ2" s="43" t="s">
+      <c r="AO2" s="43" t="s">
         <v>252</v>
       </c>
-      <c r="AK2" s="43" t="s">
+      <c r="AP2" s="43" t="s">
         <v>253</v>
       </c>
-      <c r="AL2" s="43" t="s">
+      <c r="AQ2" s="43" t="s">
         <v>254</v>
-      </c>
-      <c r="AM2" s="43" t="s">
-        <v>255</v>
-      </c>
-      <c r="AN2" s="43" t="s">
-        <v>256</v>
-      </c>
-      <c r="AO2" s="43" t="s">
-        <v>257</v>
-      </c>
-      <c r="AP2" s="43" t="s">
-        <v>258</v>
-      </c>
-      <c r="AQ2" s="43" t="s">
-        <v>259</v>
       </c>
       <c r="AR2" s="45" t="s">
         <v>87</v>
@@ -4867,37 +4718,37 @@
         <v>93</v>
       </c>
       <c r="AY2" s="45" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="AZ2" s="45" t="s">
         <v>94</v>
       </c>
       <c r="BA2" s="47" t="s">
+        <v>256</v>
+      </c>
+      <c r="BB2" s="47" t="s">
+        <v>257</v>
+      </c>
+      <c r="BC2" s="47" t="s">
+        <v>258</v>
+      </c>
+      <c r="BD2" s="47" t="s">
+        <v>259</v>
+      </c>
+      <c r="BE2" s="47" t="s">
+        <v>260</v>
+      </c>
+      <c r="BF2" s="49" t="s">
         <v>261</v>
       </c>
-      <c r="BB2" s="47" t="s">
+      <c r="BG2" s="49" t="s">
         <v>262</v>
       </c>
-      <c r="BC2" s="47" t="s">
+      <c r="BH2" s="49" t="s">
         <v>263</v>
       </c>
-      <c r="BD2" s="47" t="s">
+      <c r="BI2" s="49" t="s">
         <v>264</v>
-      </c>
-      <c r="BE2" s="47" t="s">
-        <v>265</v>
-      </c>
-      <c r="BF2" s="49" t="s">
-        <v>266</v>
-      </c>
-      <c r="BG2" s="49" t="s">
-        <v>267</v>
-      </c>
-      <c r="BH2" s="49" t="s">
-        <v>268</v>
-      </c>
-      <c r="BI2" s="49" t="s">
-        <v>269</v>
       </c>
       <c r="BJ2" s="51" t="s">
         <v>105</v>
@@ -4909,70 +4760,70 @@
         <v>107</v>
       </c>
       <c r="BM2" s="53" t="s">
+        <v>265</v>
+      </c>
+      <c r="BN2" s="53" t="s">
+        <v>266</v>
+      </c>
+      <c r="BO2" s="53" t="s">
+        <v>267</v>
+      </c>
+      <c r="BP2" s="53" t="s">
+        <v>268</v>
+      </c>
+      <c r="BQ2" s="53" t="s">
+        <v>269</v>
+      </c>
+      <c r="BR2" s="53" t="s">
         <v>270</v>
       </c>
-      <c r="BN2" s="53" t="s">
+      <c r="BS2" s="53" t="s">
         <v>271</v>
       </c>
-      <c r="BO2" s="53" t="s">
+      <c r="BT2" s="55" t="s">
+        <v>265</v>
+      </c>
+      <c r="BU2" s="55" t="s">
         <v>272</v>
       </c>
-      <c r="BP2" s="53" t="s">
+      <c r="BV2" s="55" t="s">
+        <v>268</v>
+      </c>
+      <c r="BW2" s="55" t="s">
         <v>273</v>
       </c>
-      <c r="BQ2" s="53" t="s">
+      <c r="BX2" s="55" t="s">
+        <v>269</v>
+      </c>
+      <c r="BY2" s="55" t="s">
         <v>274</v>
       </c>
-      <c r="BR2" s="53" t="s">
+      <c r="BZ2" s="57" t="s">
         <v>275</v>
       </c>
-      <c r="BS2" s="53" t="s">
+      <c r="CA2" s="57" t="s">
         <v>276</v>
       </c>
-      <c r="BT2" s="55" t="s">
-        <v>270</v>
-      </c>
-      <c r="BU2" s="55" t="s">
+      <c r="CB2" s="57" t="s">
         <v>277</v>
       </c>
-      <c r="BV2" s="55" t="s">
-        <v>273</v>
-      </c>
-      <c r="BW2" s="55" t="s">
+      <c r="CC2" s="58" t="s">
         <v>278</v>
       </c>
-      <c r="BX2" s="55" t="s">
-        <v>274</v>
-      </c>
-      <c r="BY2" s="55" t="s">
+      <c r="CD2" s="59" t="s">
+        <v>265</v>
+      </c>
+      <c r="CE2" s="59" t="s">
+        <v>272</v>
+      </c>
+      <c r="CF2" s="59" t="s">
         <v>279</v>
       </c>
-      <c r="BZ2" s="57" t="s">
+      <c r="CG2" s="59" t="s">
+        <v>269</v>
+      </c>
+      <c r="CH2" s="59" t="s">
         <v>280</v>
-      </c>
-      <c r="CA2" s="57" t="s">
-        <v>281</v>
-      </c>
-      <c r="CB2" s="57" t="s">
-        <v>282</v>
-      </c>
-      <c r="CC2" s="58" t="s">
-        <v>283</v>
-      </c>
-      <c r="CD2" s="59" t="s">
-        <v>270</v>
-      </c>
-      <c r="CE2" s="59" t="s">
-        <v>277</v>
-      </c>
-      <c r="CF2" s="59" t="s">
-        <v>284</v>
-      </c>
-      <c r="CG2" s="59" t="s">
-        <v>274</v>
-      </c>
-      <c r="CH2" s="59" t="s">
-        <v>285</v>
       </c>
       <c r="CI2" s="61" t="s">
         <v>108</v>
@@ -4981,7 +4832,7 @@
         <v>109</v>
       </c>
       <c r="CK2" s="61" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="CL2" s="61" t="s">
         <v>111</v>
@@ -4993,7 +4844,7 @@
         <v>113</v>
       </c>
       <c r="CO2" s="63" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="CP2" s="63" t="s">
         <v>116</v>
@@ -5002,82 +4853,82 @@
         <v>117</v>
       </c>
       <c r="CR2" s="65" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="CS2" s="65" t="s">
+        <v>280</v>
+      </c>
+      <c r="CT2" s="65" t="s">
+        <v>280</v>
+      </c>
+      <c r="CU2" s="65" t="s">
+        <v>283</v>
+      </c>
+      <c r="CV2" s="67" t="s">
+        <v>284</v>
+      </c>
+      <c r="CW2" s="67" t="s">
         <v>285</v>
       </c>
-      <c r="CT2" s="65" t="s">
-        <v>285</v>
-      </c>
-      <c r="CU2" s="65" t="s">
+      <c r="CX2" s="67" t="s">
+        <v>286</v>
+      </c>
+      <c r="CY2" s="67" t="s">
+        <v>287</v>
+      </c>
+      <c r="CZ2" s="67" t="s">
         <v>288</v>
       </c>
-      <c r="CV2" s="67" t="s">
+      <c r="DA2" s="67" t="s">
         <v>289</v>
       </c>
-      <c r="CW2" s="67" t="s">
+      <c r="DB2" s="67" t="s">
         <v>290</v>
       </c>
-      <c r="CX2" s="67" t="s">
+      <c r="DC2" s="67" t="s">
         <v>291</v>
       </c>
-      <c r="CY2" s="67" t="s">
+      <c r="DD2" s="67" t="s">
         <v>292</v>
       </c>
-      <c r="CZ2" s="67" t="s">
+      <c r="DE2" s="90" t="s">
+        <v>272</v>
+      </c>
+      <c r="DF2" s="90" t="s">
         <v>293</v>
       </c>
-      <c r="DA2" s="67" t="s">
+      <c r="DG2" s="90" t="s">
+        <v>280</v>
+      </c>
+      <c r="DH2" s="90" t="s">
+        <v>274</v>
+      </c>
+      <c r="DI2" s="90" t="s">
         <v>294</v>
       </c>
-      <c r="DB2" s="67" t="s">
+      <c r="DJ2" s="90" t="s">
         <v>295</v>
       </c>
-      <c r="DC2" s="67" t="s">
+      <c r="DK2" s="90" t="s">
         <v>296</v>
       </c>
-      <c r="DD2" s="67" t="s">
+      <c r="DL2" s="90" t="s">
         <v>297</v>
       </c>
-      <c r="DE2" s="90" t="s">
-        <v>277</v>
-      </c>
-      <c r="DF2" s="90" t="s">
+      <c r="DM2" s="90" t="s">
         <v>298</v>
       </c>
-      <c r="DG2" s="90" t="s">
-        <v>285</v>
-      </c>
-      <c r="DH2" s="90" t="s">
-        <v>279</v>
-      </c>
-      <c r="DI2" s="90" t="s">
+      <c r="DN2" s="90" t="s">
         <v>299</v>
       </c>
-      <c r="DJ2" s="90" t="s">
+      <c r="DO2" s="90" t="s">
         <v>300</v>
       </c>
-      <c r="DK2" s="90" t="s">
+      <c r="DP2" s="90" t="s">
         <v>301</v>
       </c>
-      <c r="DL2" s="90" t="s">
+      <c r="DQ2" s="90" t="s">
         <v>302</v>
-      </c>
-      <c r="DM2" s="90" t="s">
-        <v>303</v>
-      </c>
-      <c r="DN2" s="90" t="s">
-        <v>304</v>
-      </c>
-      <c r="DO2" s="90" t="s">
-        <v>305</v>
-      </c>
-      <c r="DP2" s="90" t="s">
-        <v>306</v>
-      </c>
-      <c r="DQ2" s="90" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="3" spans="1:121" ht="52.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5185,7 +5036,7 @@
         <v>25</v>
       </c>
       <c r="AJ3" s="43" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="AK3" s="43" t="s">
         <v>121</v>
@@ -5244,7 +5095,7 @@
         <v>124</v>
       </c>
       <c r="BE3" s="47" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="BF3" s="49" t="s">
         <v>20</v>
@@ -5268,7 +5119,7 @@
         <v>124</v>
       </c>
       <c r="BM3" s="53" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="BN3" s="53" t="s">
         <v>23</v>
@@ -5298,7 +5149,7 @@
         <v>20</v>
       </c>
       <c r="BW3" s="55" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="BX3" s="55" t="s">
         <v>124</v>
@@ -5316,7 +5167,7 @@
         <v>124</v>
       </c>
       <c r="CC3" s="58" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="CD3" s="59" t="s">
         <v>120</v>
@@ -5370,13 +5221,13 @@
         <v>28</v>
       </c>
       <c r="CU3" s="65" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="CV3" s="67" t="s">
         <v>121</v>
       </c>
       <c r="CW3" s="67" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="CX3" s="67" t="s">
         <v>121</v>
@@ -5415,25 +5266,25 @@
         <v>121</v>
       </c>
       <c r="DJ3" s="90" t="s">
+        <v>303</v>
+      </c>
+      <c r="DK3" s="90" t="s">
+        <v>307</v>
+      </c>
+      <c r="DL3" s="90" t="s">
         <v>308</v>
       </c>
-      <c r="DK3" s="90" t="s">
-        <v>312</v>
-      </c>
-      <c r="DL3" s="90" t="s">
-        <v>313</v>
-      </c>
       <c r="DM3" s="90" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="DN3" s="90" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="DO3" s="90" t="s">
         <v>124</v>
       </c>
       <c r="DP3" s="90" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="DQ3" s="90" t="s">
         <v>20</v>
@@ -5480,10 +5331,10 @@
       <c r="V4" s="36"/>
       <c r="W4" s="36"/>
       <c r="X4" s="38" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="Y4" s="38" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="Z4" s="37" t="s">
         <v>131</v>
@@ -5493,7 +5344,7 @@
       <c r="AC4" s="40"/>
       <c r="AD4" s="40"/>
       <c r="AE4" s="42" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="AF4" s="42"/>
       <c r="AG4" s="41" t="s">
@@ -5504,7 +5355,7 @@
       <c r="AJ4" s="44"/>
       <c r="AK4" s="44"/>
       <c r="AL4" s="43" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="AM4" s="43"/>
       <c r="AN4" s="43" t="s">
@@ -5527,33 +5378,33 @@
       <c r="AW4" s="46"/>
       <c r="AX4" s="46"/>
       <c r="AY4" s="46" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="AZ4" s="46" t="s">
         <v>137</v>
       </c>
       <c r="BA4" s="48" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="BB4" s="48" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="BC4" s="48" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="BD4" s="48"/>
       <c r="BE4" s="48"/>
       <c r="BF4" s="50" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="BG4" s="50" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="BH4" s="50" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="BI4" s="50" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="BJ4" s="52" t="s">
         <v>139</v>
@@ -5564,47 +5415,47 @@
       <c r="BL4" s="52"/>
       <c r="BM4" s="54"/>
       <c r="BN4" s="54" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="BO4" s="54" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="BP4" s="54" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="BQ4" s="54"/>
       <c r="BR4" s="54"/>
       <c r="BS4" s="54"/>
       <c r="BT4" s="56" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="BU4" s="56" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="BV4" s="56" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="BW4" s="56"/>
       <c r="BX4" s="56"/>
       <c r="BY4" s="56" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="BZ4" s="58" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="CA4" s="58" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="CB4" s="58"/>
       <c r="CC4" s="58"/>
       <c r="CD4" s="60" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="CE4" s="60" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="CF4" s="60" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="CG4" s="59"/>
       <c r="CH4" s="59"/>
@@ -5640,10 +5491,10 @@
       <c r="DB4" s="68"/>
       <c r="DC4" s="68"/>
       <c r="DD4" s="68" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="DE4" s="90" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="DF4" s="90"/>
       <c r="DG4" s="90"/>
@@ -5729,62 +5580,62 @@
         <v>42</v>
       </c>
       <c r="X5" s="37" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="Y5" s="37" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="Z5" s="37" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="AA5" s="37" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="AB5" s="39" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="AC5" s="39" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="AD5" s="39" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="AE5" s="42" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="AF5" s="41" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="AG5" s="41" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="AH5" s="41" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="AI5" s="41"/>
       <c r="AJ5" s="43" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="AK5" s="43" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="AL5" s="44" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="AM5" s="43" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="AN5" s="43" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="AO5" s="43" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="AP5" s="43" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="AQ5" s="43" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="AR5" s="45" t="s">
         <v>39</v>
@@ -5814,28 +5665,28 @@
         <v>39</v>
       </c>
       <c r="BA5" s="48" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="BB5" s="47" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="BC5" s="47" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="BD5" s="47" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="BE5" s="47" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="BF5" s="50" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="BG5" s="49" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="BH5" s="49" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="BI5" s="49"/>
       <c r="BJ5" s="52" t="s">
@@ -5848,82 +5699,82 @@
         <v>47</v>
       </c>
       <c r="BM5" s="54" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="BN5" s="54" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="BO5" s="54" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="BP5" s="54" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="BQ5" s="54" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="BR5" s="54" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="BS5" s="53" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="BT5" s="55" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="BU5" s="55" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="BV5" s="55" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="BW5" s="55" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="BX5" s="56" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="BY5" s="55" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="BZ5" s="58" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="CA5" s="57" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="CB5" s="57" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="CC5" s="58" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="CD5" s="60" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="CE5" s="59" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="CF5" s="59" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="CG5" s="59" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="CH5" s="59" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="CI5" s="61" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="CJ5" s="61" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="CK5" s="61" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="CL5" s="61" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="CM5" s="61"/>
       <c r="CN5" s="63" t="s">
@@ -5939,82 +5790,82 @@
         <v>55</v>
       </c>
       <c r="CR5" s="66" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="CS5" s="66" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="CT5" s="65" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="CU5" s="65" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="CV5" s="67" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="CW5" s="67" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="CX5" s="67" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="CY5" s="67" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="CZ5" s="67" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="DA5" s="67" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="DB5" s="67" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="DC5" s="67" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="DD5" s="67" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="DE5" s="90" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="DF5" s="90" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="DG5" s="90" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="DH5" s="90" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="DI5" s="90" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="DJ5" s="90" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="DK5" s="90" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="DL5" s="90" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="DM5" s="90" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="DN5" s="90" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="DO5" s="90" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="DP5" s="90" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="DQ5" s="90" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
     </row>
     <row r="6" spans="1:121" s="2" customFormat="1" ht="52.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6085,67 +5936,67 @@
         <v>168</v>
       </c>
       <c r="W6" s="88" t="s">
+        <v>348</v>
+      </c>
+      <c r="X6" s="88" t="s">
+        <v>349</v>
+      </c>
+      <c r="Y6" s="88" t="s">
+        <v>350</v>
+      </c>
+      <c r="Z6" s="88" t="s">
+        <v>351</v>
+      </c>
+      <c r="AA6" s="88" t="s">
+        <v>352</v>
+      </c>
+      <c r="AB6" s="88" t="s">
         <v>353</v>
       </c>
-      <c r="X6" s="88" t="s">
+      <c r="AC6" s="88" t="s">
         <v>354</v>
       </c>
-      <c r="Y6" s="88" t="s">
+      <c r="AD6" s="88" t="s">
         <v>355</v>
       </c>
-      <c r="Z6" s="88" t="s">
+      <c r="AE6" s="88" t="s">
         <v>356</v>
       </c>
-      <c r="AA6" s="88" t="s">
+      <c r="AF6" s="88" t="s">
         <v>357</v>
       </c>
-      <c r="AB6" s="88" t="s">
+      <c r="AG6" s="88" t="s">
         <v>358</v>
       </c>
-      <c r="AC6" s="88" t="s">
+      <c r="AH6" s="88" t="s">
         <v>359</v>
       </c>
-      <c r="AD6" s="88" t="s">
+      <c r="AI6" s="88" t="s">
         <v>360</v>
       </c>
-      <c r="AE6" s="88" t="s">
+      <c r="AJ6" s="88" t="s">
         <v>361</v>
       </c>
-      <c r="AF6" s="88" t="s">
+      <c r="AK6" s="88" t="s">
         <v>362</v>
       </c>
-      <c r="AG6" s="88" t="s">
+      <c r="AL6" s="88" t="s">
         <v>363</v>
       </c>
-      <c r="AH6" s="88" t="s">
+      <c r="AM6" s="88" t="s">
         <v>364</v>
       </c>
-      <c r="AI6" s="88" t="s">
+      <c r="AN6" s="88" t="s">
         <v>365</v>
       </c>
-      <c r="AJ6" s="88" t="s">
+      <c r="AO6" s="88" t="s">
         <v>366</v>
       </c>
-      <c r="AK6" s="88" t="s">
+      <c r="AP6" s="88" t="s">
         <v>367</v>
       </c>
-      <c r="AL6" s="88" t="s">
+      <c r="AQ6" s="88" t="s">
         <v>368</v>
-      </c>
-      <c r="AM6" s="88" t="s">
-        <v>369</v>
-      </c>
-      <c r="AN6" s="88" t="s">
-        <v>370</v>
-      </c>
-      <c r="AO6" s="88" t="s">
-        <v>371</v>
-      </c>
-      <c r="AP6" s="88" t="s">
-        <v>372</v>
-      </c>
-      <c r="AQ6" s="88" t="s">
-        <v>373</v>
       </c>
       <c r="AR6" s="88" t="s">
         <v>170</v>
@@ -6169,37 +6020,37 @@
         <v>176</v>
       </c>
       <c r="AY6" s="88" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="AZ6" s="88" t="s">
         <v>177</v>
       </c>
       <c r="BA6" s="88" t="s">
+        <v>370</v>
+      </c>
+      <c r="BB6" s="88" t="s">
+        <v>371</v>
+      </c>
+      <c r="BC6" s="88" t="s">
+        <v>372</v>
+      </c>
+      <c r="BD6" s="88" t="s">
+        <v>373</v>
+      </c>
+      <c r="BE6" s="88" t="s">
+        <v>374</v>
+      </c>
+      <c r="BF6" s="88" t="s">
         <v>375</v>
       </c>
-      <c r="BB6" s="88" t="s">
+      <c r="BG6" s="88" t="s">
         <v>376</v>
       </c>
-      <c r="BC6" s="88" t="s">
+      <c r="BH6" s="88" t="s">
         <v>377</v>
       </c>
-      <c r="BD6" s="88" t="s">
+      <c r="BI6" s="88" t="s">
         <v>378</v>
-      </c>
-      <c r="BE6" s="88" t="s">
-        <v>379</v>
-      </c>
-      <c r="BF6" s="88" t="s">
-        <v>380</v>
-      </c>
-      <c r="BG6" s="88" t="s">
-        <v>381</v>
-      </c>
-      <c r="BH6" s="88" t="s">
-        <v>382</v>
-      </c>
-      <c r="BI6" s="88" t="s">
-        <v>383</v>
       </c>
       <c r="BJ6" s="88" t="s">
         <v>188</v>
@@ -6211,70 +6062,70 @@
         <v>190</v>
       </c>
       <c r="BM6" s="88" t="s">
+        <v>379</v>
+      </c>
+      <c r="BN6" s="88" t="s">
+        <v>380</v>
+      </c>
+      <c r="BO6" s="88" t="s">
+        <v>381</v>
+      </c>
+      <c r="BP6" s="88" t="s">
+        <v>382</v>
+      </c>
+      <c r="BQ6" s="88" t="s">
+        <v>383</v>
+      </c>
+      <c r="BR6" s="88" t="s">
         <v>384</v>
       </c>
-      <c r="BN6" s="88" t="s">
+      <c r="BS6" s="88" t="s">
         <v>385</v>
       </c>
-      <c r="BO6" s="88" t="s">
+      <c r="BT6" s="88" t="s">
         <v>386</v>
       </c>
-      <c r="BP6" s="88" t="s">
+      <c r="BU6" s="88" t="s">
         <v>387</v>
       </c>
-      <c r="BQ6" s="88" t="s">
+      <c r="BV6" s="88" t="s">
         <v>388</v>
       </c>
-      <c r="BR6" s="88" t="s">
+      <c r="BW6" s="88" t="s">
         <v>389</v>
       </c>
-      <c r="BS6" s="88" t="s">
+      <c r="BX6" s="88" t="s">
+        <v>383</v>
+      </c>
+      <c r="BY6" s="88" t="s">
         <v>390</v>
       </c>
-      <c r="BT6" s="88" t="s">
+      <c r="BZ6" s="88" t="s">
         <v>391</v>
       </c>
-      <c r="BU6" s="88" t="s">
+      <c r="CA6" s="88" t="s">
         <v>392</v>
       </c>
-      <c r="BV6" s="88" t="s">
+      <c r="CB6" s="88" t="s">
         <v>393</v>
       </c>
-      <c r="BW6" s="88" t="s">
+      <c r="CC6" s="88" t="s">
         <v>394</v>
       </c>
-      <c r="BX6" s="88" t="s">
-        <v>388</v>
-      </c>
-      <c r="BY6" s="88" t="s">
+      <c r="CD6" s="88" t="s">
         <v>395</v>
       </c>
-      <c r="BZ6" s="88" t="s">
+      <c r="CE6" s="88" t="s">
         <v>396</v>
       </c>
-      <c r="CA6" s="88" t="s">
+      <c r="CF6" s="88" t="s">
+        <v>382</v>
+      </c>
+      <c r="CG6" s="88" t="s">
         <v>397</v>
       </c>
-      <c r="CB6" s="88" t="s">
+      <c r="CH6" s="88" t="s">
         <v>398</v>
-      </c>
-      <c r="CC6" s="88" t="s">
-        <v>399</v>
-      </c>
-      <c r="CD6" s="88" t="s">
-        <v>400</v>
-      </c>
-      <c r="CE6" s="88" t="s">
-        <v>401</v>
-      </c>
-      <c r="CF6" s="88" t="s">
-        <v>387</v>
-      </c>
-      <c r="CG6" s="88" t="s">
-        <v>402</v>
-      </c>
-      <c r="CH6" s="88" t="s">
-        <v>403</v>
       </c>
       <c r="CI6" s="88" t="s">
         <v>191</v>
@@ -6304,80 +6155,80 @@
         <v>200</v>
       </c>
       <c r="CR6" s="88" t="s">
+        <v>399</v>
+      </c>
+      <c r="CS6" s="88" t="s">
+        <v>400</v>
+      </c>
+      <c r="CT6" s="88" t="s">
+        <v>401</v>
+      </c>
+      <c r="CU6" s="88" t="s">
+        <v>402</v>
+      </c>
+      <c r="CV6" s="88" t="s">
+        <v>403</v>
+      </c>
+      <c r="CW6" s="88" t="s">
         <v>404</v>
       </c>
-      <c r="CS6" s="88" t="s">
+      <c r="CX6" s="88" t="s">
         <v>405</v>
       </c>
-      <c r="CT6" s="88" t="s">
+      <c r="CY6" s="88" t="s">
         <v>406</v>
       </c>
-      <c r="CU6" s="88" t="s">
+      <c r="CZ6" s="88" t="s">
         <v>407</v>
       </c>
-      <c r="CV6" s="88" t="s">
+      <c r="DA6" s="88" t="s">
         <v>408</v>
       </c>
-      <c r="CW6" s="88" t="s">
+      <c r="DB6" s="88" t="s">
         <v>409</v>
       </c>
-      <c r="CX6" s="88" t="s">
+      <c r="DC6" s="88" t="s">
         <v>410</v>
-      </c>
-      <c r="CY6" s="88" t="s">
-        <v>411</v>
-      </c>
-      <c r="CZ6" s="88" t="s">
-        <v>412</v>
-      </c>
-      <c r="DA6" s="88" t="s">
-        <v>413</v>
-      </c>
-      <c r="DB6" s="88" t="s">
-        <v>414</v>
-      </c>
-      <c r="DC6" s="88" t="s">
-        <v>415</v>
       </c>
       <c r="DD6" s="89"/>
       <c r="DE6" s="89" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="DF6" s="89" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="DG6" s="89" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="DH6" s="89" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="DI6" s="89" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="DJ6" s="89" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="DK6" s="89" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="DL6" s="89" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="DM6" s="89" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="DN6" s="89" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="DO6" s="89" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="DP6" s="89" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="DQ6" s="89" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
     </row>
     <row r="7" spans="1:121" ht="16" x14ac:dyDescent="0.2">
@@ -6477,7 +6328,7 @@
       <c r="CP7" s="16"/>
       <c r="CQ7" s="16"/>
       <c r="CR7" s="96" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="CS7" s="16"/>
       <c r="CT7" s="16"/>

</xml_diff>